<commit_message>
menghapus perbedaan harga toko dan pelanggan
</commit_message>
<xml_diff>
--- a/storage/app/public/assets/format_produk.xlsx
+++ b/storage/app/public/assets/format_produk.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\servis-online\storage\app\public\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\servis-online\public\storage\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB07B7A0-A0BE-40C7-8A5A-A75FC2E346AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201B2423-FFB5-48A7-B331-940714D108CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Nama Produk</t>
   </si>
@@ -40,16 +40,13 @@
     <t>Harga Modal</t>
   </si>
   <si>
-    <t>Harga Pelanggan</t>
-  </si>
-  <si>
-    <t>Harga Toko</t>
-  </si>
-  <si>
     <t>Keterangan</t>
   </si>
   <si>
     <t>Agen</t>
+  </si>
+  <si>
+    <t>Harga Jual</t>
   </si>
 </sst>
 </file>
@@ -417,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -431,11 +428,11 @@
     <col min="4" max="4" width="19.109375" customWidth="1"/>
     <col min="5" max="5" width="9.5546875" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="9" width="16.33203125" customWidth="1"/>
-    <col min="10" max="10" width="19.44140625" customWidth="1"/>
+    <col min="7" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="9" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -454,23 +451,20 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
update format excel produk
</commit_message>
<xml_diff>
--- a/storage/app/public/assets/format_produk.xlsx
+++ b/storage/app/public/assets/format_produk.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\servis-online\public\storage\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\servis-online\storage\app\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201B2423-FFB5-48A7-B331-940714D108CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C1D585B-9930-485A-A816-F490F3AD89A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Nama Produk</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Nomor Seri</t>
   </si>
   <si>
-    <t>ID Kategori</t>
-  </si>
-  <si>
     <t>Stok</t>
   </si>
   <si>
@@ -47,13 +44,28 @@
   </si>
   <si>
     <t>Harga Jual</t>
+  </si>
+  <si>
+    <t>ID Sub Kategori</t>
+  </si>
+  <si>
+    <t>Nama Sub Kategori</t>
+  </si>
+  <si>
+    <t>Garansi IMEI</t>
+  </si>
+  <si>
+    <t>PPN 11%</t>
+  </si>
+  <si>
+    <t>Garansi Produk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -68,12 +80,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -105,10 +111,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -414,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -425,14 +430,16 @@
     <col min="1" max="1" width="55.21875" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="8" width="16.33203125" customWidth="1"/>
-    <col min="9" max="9" width="19.44140625" customWidth="1"/>
+    <col min="4" max="5" width="19.109375" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="8" max="9" width="16.33203125" customWidth="1"/>
+    <col min="10" max="10" width="19.44140625" customWidth="1"/>
+    <col min="11" max="11" width="14.44140625" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,28 +450,35 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="J1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
update format produk excel
</commit_message>
<xml_diff>
--- a/storage/app/public/assets/format_produk.xlsx
+++ b/storage/app/public/assets/format_produk.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\servis-online\public\storage\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khaed\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5E28DE-4600-4B40-987B-FD3E9DBD8505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEA8BBB-E7A7-4D2B-98D4-15C4CDA9CA94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Nama Produk</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Nomor Seri</t>
   </si>
   <si>
-    <t>ID Kategori</t>
-  </si>
-  <si>
     <t>Stok</t>
   </si>
   <si>
@@ -47,13 +44,28 @@
   </si>
   <si>
     <t>Harga Jual</t>
+  </si>
+  <si>
+    <t>ID Sub Kategori</t>
+  </si>
+  <si>
+    <t>Nama Sub Kategori</t>
+  </si>
+  <si>
+    <t>Garansi IMEI</t>
+  </si>
+  <si>
+    <t>PPN 11%</t>
+  </si>
+  <si>
+    <t>Garansi Produk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -68,12 +80,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -105,10 +111,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -414,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -425,14 +430,16 @@
     <col min="1" max="1" width="55.21875" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="8" width="16.33203125" customWidth="1"/>
-    <col min="9" max="9" width="19.44140625" customWidth="1"/>
+    <col min="4" max="5" width="19.109375" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="8" max="9" width="16.33203125" customWidth="1"/>
+    <col min="10" max="10" width="19.44140625" customWidth="1"/>
+    <col min="11" max="11" width="14.44140625" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,28 +450,35 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="J1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
hapus field supplier pada produk
</commit_message>
<xml_diff>
--- a/storage/app/public/assets/format_produk.xlsx
+++ b/storage/app/public/assets/format_produk.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\servis-online\storage\app\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C1D585B-9930-485A-A816-F490F3AD89A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACF2920-E90C-4348-8019-3F8152D47CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Nama Produk</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t>Keterangan</t>
-  </si>
-  <si>
-    <t>Agen</t>
   </si>
   <si>
     <t>Harga Jual</t>
@@ -419,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -433,13 +430,13 @@
     <col min="4" max="5" width="19.109375" customWidth="1"/>
     <col min="6" max="6" width="9.5546875" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" customWidth="1"/>
-    <col min="8" max="9" width="16.33203125" customWidth="1"/>
-    <col min="10" max="10" width="19.44140625" customWidth="1"/>
-    <col min="11" max="11" width="14.44140625" customWidth="1"/>
-    <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="9" width="19.44140625" customWidth="1"/>
+    <col min="10" max="10" width="14.44140625" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -450,10 +447,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -462,22 +459,19 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="K1" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add input stok minimal produk
</commit_message>
<xml_diff>
--- a/storage/app/public/assets/format_produk.xlsx
+++ b/storage/app/public/assets/format_produk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\servis-online\storage\app\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACF2920-E90C-4348-8019-3F8152D47CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAD5941-D35A-431E-8260-D973D1A628EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-132" yWindow="-132" windowWidth="23304" windowHeight="12504" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Nama Produk</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>Garansi Produk</t>
+  </si>
+  <si>
+    <t>Stok Minimal</t>
   </si>
 </sst>
 </file>
@@ -416,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -429,14 +432,15 @@
     <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="19.109375" customWidth="1"/>
     <col min="6" max="6" width="9.5546875" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" customWidth="1"/>
-    <col min="9" max="9" width="19.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" customWidth="1"/>
-    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" customWidth="1"/>
+    <col min="10" max="10" width="19.44140625" customWidth="1"/>
+    <col min="11" max="11" width="14.44140625" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -456,21 +460,24 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>